<commit_message>
Update testcases.xlsx to reflect changes in DCC cases handling
</commit_message>
<xml_diff>
--- a/testcases.xlsx
+++ b/testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energinet-my.sharepoint.com/personal/prw_energinet_dk/Documents/Dokumenter/GitHub/MTB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="11_75BCC0E3648942E3F9B3ABC73D174D462146C19F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D55F73F-7687-4A56-9060-6B99955C88B8}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="11_75BCC0E3648942E3F9B3ABC73D174D462146C19F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2822A63F-9E62-5889-8F7B-BDC091F69563}"/>
   <bookViews>
-    <workbookView xWindow="-17610" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="822" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14480" yWindow="-21710" windowWidth="51420" windowHeight="21100" tabRatio="822" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -53446,6 +53446,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="C2:C11"/>
+    <mergeCell ref="C12:C17"/>
+    <mergeCell ref="C18:C28"/>
+    <mergeCell ref="C44:C53"/>
+    <mergeCell ref="C29:C43"/>
     <mergeCell ref="C163:C176"/>
     <mergeCell ref="C61:C70"/>
     <mergeCell ref="C71:C94"/>
@@ -53453,13 +53460,6 @@
     <mergeCell ref="C99:C108"/>
     <mergeCell ref="C109:C115"/>
     <mergeCell ref="C116:C162"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="C2:C11"/>
-    <mergeCell ref="C12:C17"/>
-    <mergeCell ref="C18:C28"/>
-    <mergeCell ref="C44:C53"/>
-    <mergeCell ref="C29:C43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -53996,6 +53996,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="107e75b3-53cc-4838-92d2-ebc011bd4832">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="888ccf44-0d39-41a2-ab17-f7efb2bf6977" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004FD8CECCB51EC843BF514AFE68379818" ma:contentTypeVersion="18" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="eda339f53f012ceb64677667a741b441">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="107e75b3-53cc-4838-92d2-ebc011bd4832" xmlns:ns3="888ccf44-0d39-41a2-ab17-f7efb2bf6977" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="04a86f3db711706e561c315688f1c464" ns2:_="" ns3:_="">
     <xsd:import namespace="107e75b3-53cc-4838-92d2-ebc011bd4832"/>
@@ -54244,17 +54255,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="107e75b3-53cc-4838-92d2-ebc011bd4832">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="888ccf44-0d39-41a2-ab17-f7efb2bf6977" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74B21D61-7BBD-4BD3-A9A5-1E8F98F2F686}">
   <ds:schemaRefs>
@@ -54264,6 +54264,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2288FB7-E85A-4FE8-9E7A-FE572FF16064}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="888ccf44-0d39-41a2-ab17-f7efb2bf6977"/>
+    <ds:schemaRef ds:uri="107e75b3-53cc-4838-92d2-ebc011bd4832"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F91B7B9-75FF-4624-B506-952B5B54766C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -54280,21 +54297,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2288FB7-E85A-4FE8-9E7A-FE572FF16064}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="888ccf44-0d39-41a2-ab17-f7efb2bf6977"/>
-    <ds:schemaRef ds:uri="107e75b3-53cc-4838-92d2-ebc011bd4832"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>